<commit_message>
added fix and implementation for filtering data by year in employee_details
</commit_message>
<xml_diff>
--- a/python_source/hr_ptcc_project/static/employee_profile/files/generated_leave_registry_2020.xlsx
+++ b/python_source/hr_ptcc_project/static/employee_profile/files/generated_leave_registry_2020.xlsx
@@ -1606,7 +1606,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>June 02, 2020</t>
+          <t>June 03, 2020</t>
         </is>
       </c>
     </row>
@@ -1618,7 +1618,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>June 02, 2020</t>
+          <t>June 03, 2020</t>
         </is>
       </c>
     </row>
@@ -1693,13 +1693,13 @@
         </is>
       </c>
       <c r="G13" s="70" t="n">
-        <v>5</v>
+        <v>5.625</v>
       </c>
       <c r="H13" s="71" t="n">
         <v>0.5</v>
       </c>
       <c r="I13" s="72" t="n">
-        <v>4.5</v>
+        <v>5.125</v>
       </c>
     </row>
     <row customHeight="1" ht="15.8" r="14" s="50">
@@ -1713,13 +1713,13 @@
         </is>
       </c>
       <c r="G14" s="77" t="n">
-        <v>3.328</v>
+        <v>3.744</v>
       </c>
       <c r="H14" s="78" t="n">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="I14" s="79" t="n">
-        <v>3.328</v>
+        <v>-0.7560000000000002</v>
       </c>
     </row>
     <row customHeight="1" ht="15.8" r="15" s="50">
@@ -1818,16 +1818,16 @@
       </c>
       <c r="F19" s="87" t="inlineStr">
         <is>
-          <t>May 20, 2020</t>
+          <t>May 19, 2020</t>
         </is>
       </c>
       <c r="G19" s="88" t="n">
-        <v>0.5</v>
+        <v>4.5</v>
       </c>
       <c r="H19" s="89" t="n"/>
       <c r="I19" s="90" t="inlineStr">
         <is>
-          <t>VL</t>
+          <t>SL</t>
         </is>
       </c>
     </row>
@@ -1844,10 +1844,20 @@
       <c r="D20" s="83" t="n">
         <v>0.416</v>
       </c>
-      <c r="F20" s="87" t="n"/>
-      <c r="G20" s="88" t="n"/>
+      <c r="F20" s="87" t="inlineStr">
+        <is>
+          <t>May 20, 2020</t>
+        </is>
+      </c>
+      <c r="G20" s="88" t="n">
+        <v>0.5</v>
+      </c>
       <c r="H20" s="89" t="n"/>
-      <c r="I20" s="90" t="n"/>
+      <c r="I20" s="90" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15.8" r="21" s="50">
       <c r="A21" s="73" t="n">
@@ -1911,10 +1921,10 @@
         <v>43966</v>
       </c>
       <c r="C24" s="82" t="n">
-        <v>0</v>
+        <v>0.625</v>
       </c>
       <c r="D24" s="83" t="n">
-        <v>0</v>
+        <v>0.416</v>
       </c>
       <c r="F24" s="87" t="n"/>
       <c r="G24" s="88" t="n"/>
@@ -2199,10 +2209,10 @@
         </is>
       </c>
       <c r="C40" s="93" t="n">
-        <v>5</v>
+        <v>5.625</v>
       </c>
       <c r="D40" s="94" t="n">
-        <v>3.328</v>
+        <v>3.744</v>
       </c>
       <c r="F40" s="95" t="n"/>
       <c r="G40" s="96" t="n"/>
@@ -2265,12 +2275,12 @@
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr">
         <is>
-          <t>April 12, 2020</t>
+          <t>April 13, 2020</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>No Time-out</t>
+          <t>No Time-in</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished implementation for deleting employees and adding employees.
</commit_message>
<xml_diff>
--- a/python_source/hr_ptcc_project/static/employee_profile/files/generated_leave_registry_2020.xlsx
+++ b/python_source/hr_ptcc_project/static/employee_profile/files/generated_leave_registry_2020.xlsx
@@ -1512,7 +1512,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1574,7 +1574,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>August 10, 2000</t>
+          <t>August 24, 2000</t>
         </is>
       </c>
     </row>
@@ -1585,7 +1585,7 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row customHeight="1" ht="15.8" r="7" s="50">
@@ -1606,7 +1606,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>June 03, 2020</t>
+          <t>June 04, 2020</t>
         </is>
       </c>
     </row>
@@ -1618,7 +1618,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>June 03, 2020</t>
+          <t>June 04, 2020</t>
         </is>
       </c>
     </row>
@@ -1696,10 +1696,10 @@
         <v>5.625</v>
       </c>
       <c r="H13" s="71" t="n">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="I13" s="72" t="n">
-        <v>5.125</v>
+        <v>0.625</v>
       </c>
     </row>
     <row customHeight="1" ht="15.8" r="14" s="50">
@@ -1716,10 +1716,10 @@
         <v>3.744</v>
       </c>
       <c r="H14" s="78" t="n">
-        <v>4.5</v>
+        <v>9</v>
       </c>
       <c r="I14" s="79" t="n">
-        <v>-0.7560000000000002</v>
+        <v>-5.256</v>
       </c>
     </row>
     <row customHeight="1" ht="15.8" r="15" s="50">
@@ -1730,10 +1730,10 @@
         </is>
       </c>
       <c r="C15" s="82" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D15" s="83" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row customHeight="1" ht="15.8" r="16" s="50">
@@ -1818,16 +1818,16 @@
       </c>
       <c r="F19" s="87" t="inlineStr">
         <is>
-          <t>May 19, 2020</t>
+          <t>May 26, 2020</t>
         </is>
       </c>
       <c r="G19" s="88" t="n">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="H19" s="89" t="n"/>
       <c r="I19" s="90" t="inlineStr">
         <is>
-          <t>SL</t>
+          <t>VL</t>
         </is>
       </c>
     </row>
@@ -1846,16 +1846,16 @@
       </c>
       <c r="F20" s="87" t="inlineStr">
         <is>
-          <t>May 20, 2020</t>
+          <t>June 10, 2020</t>
         </is>
       </c>
       <c r="G20" s="88" t="n">
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="H20" s="89" t="n"/>
       <c r="I20" s="90" t="inlineStr">
         <is>
-          <t>VL</t>
+          <t>SL</t>
         </is>
       </c>
     </row>
@@ -1872,10 +1872,20 @@
       <c r="D21" s="83" t="n">
         <v>0.416</v>
       </c>
-      <c r="F21" s="87" t="n"/>
-      <c r="G21" s="88" t="n"/>
+      <c r="F21" s="87" t="inlineStr">
+        <is>
+          <t>June 11, 2020</t>
+        </is>
+      </c>
+      <c r="G21" s="88" t="n">
+        <v>5</v>
+      </c>
       <c r="H21" s="89" t="n"/>
-      <c r="I21" s="90" t="n"/>
+      <c r="I21" s="90" t="inlineStr">
+        <is>
+          <t>SL</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15.8" r="22" s="50">
       <c r="A22" s="73" t="n">
@@ -2246,7 +2256,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>August 10, 2019 to August 10, 2020</t>
+          <t>August 24, 2019 to August 24, 2020</t>
         </is>
       </c>
     </row>
@@ -2275,66 +2285,46 @@
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr">
         <is>
-          <t>April 13, 2020</t>
+          <t>April 14, 2020</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
+          <t>Late</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr"/>
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>June 10, 2020</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
           <t>No Time-in</t>
         </is>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-    </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
+      <c r="A47" t="inlineStr"/>
+      <c r="B47" t="inlineStr"/>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>June 16, 2020</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>No Time-in</t>
         </is>
       </c>
     </row>
@@ -2346,27 +2336,12 @@
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr">
         <is>
-          <t xml:space="preserve">Prepared By: </t>
+          <t>June 09, 2020</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>Verified By:</t>
-        </is>
-      </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>Received By:</t>
+          <t>No Time-in</t>
         </is>
       </c>
     </row>
@@ -2432,57 +2407,143 @@
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr">
         <is>
+          <t xml:space="preserve">Prepared By: </t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Verified By:</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>Received By:</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr"/>
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="inlineStr"/>
+      <c r="F54" t="inlineStr">
+        <is>
           <t>Letecia Bodiongan</t>
         </is>
       </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
+      <c r="G54" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
         <is>
           <t>Susan Benjamin</t>
         </is>
       </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="J51" t="inlineStr">
+      <c r="I54" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
         <is>
           <t>George Smith</t>
         </is>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" t="inlineStr"/>
-      <c r="B52" t="inlineStr"/>
-      <c r="C52" t="inlineStr"/>
-      <c r="D52" t="inlineStr"/>
-      <c r="E52" t="inlineStr"/>
-      <c r="F52" t="inlineStr">
+    <row r="55">
+      <c r="A55" t="inlineStr"/>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="inlineStr"/>
+      <c r="F55" t="inlineStr">
         <is>
           <t>Accounting Supervisor - B</t>
         </is>
       </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
+      <c r="G55" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
         <is>
           <t>Finance and Admin Director</t>
         </is>
       </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="J52" t="inlineStr">
+      <c r="I55" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
         <is>
           <t>Employee</t>
         </is>

</xml_diff>

<commit_message>
fixed employee list over stretching to the footer
</commit_message>
<xml_diff>
--- a/python_source/hr_ptcc_project/static/employee_profile/files/generated_leave_registry_2020.xlsx
+++ b/python_source/hr_ptcc_project/static/employee_profile/files/generated_leave_registry_2020.xlsx
@@ -1606,7 +1606,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>June 04, 2020</t>
+          <t>June 05, 2020</t>
         </is>
       </c>
     </row>
@@ -1618,7 +1618,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>June 04, 2020</t>
+          <t>June 05, 2020</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
* separate javascript from template
* added other class methods in Employee model according to changes
</commit_message>
<xml_diff>
--- a/python_source/hr_ptcc_project/static/employee_profile/files/generated_leave_registry_2020.xlsx
+++ b/python_source/hr_ptcc_project/static/employee_profile/files/generated_leave_registry_2020.xlsx
@@ -1512,7 +1512,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1574,7 +1574,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>August 24, 2000</t>
+          <t>August 30, 2000</t>
         </is>
       </c>
     </row>
@@ -1585,7 +1585,7 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row customHeight="1" ht="15.8" r="7" s="50">
@@ -1606,7 +1606,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>June 05, 2020</t>
+          <t>June 22, 2020</t>
         </is>
       </c>
     </row>
@@ -1618,7 +1618,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>June 05, 2020</t>
+          <t>June 22, 2020</t>
         </is>
       </c>
     </row>
@@ -1693,13 +1693,13 @@
         </is>
       </c>
       <c r="G13" s="70" t="n">
-        <v>5.625</v>
+        <v>29.125</v>
       </c>
       <c r="H13" s="71" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I13" s="72" t="n">
-        <v>0.625</v>
+        <v>19.125</v>
       </c>
     </row>
     <row customHeight="1" ht="15.8" r="14" s="50">
@@ -1713,13 +1713,13 @@
         </is>
       </c>
       <c r="G14" s="77" t="n">
-        <v>3.744</v>
+        <v>26.201</v>
       </c>
       <c r="H14" s="78" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I14" s="79" t="n">
-        <v>-5.256</v>
+        <v>21.201</v>
       </c>
     </row>
     <row customHeight="1" ht="15.8" r="15" s="50">
@@ -1747,7 +1747,7 @@
         <v>0.625</v>
       </c>
       <c r="D16" s="83" t="n">
-        <v>0.416</v>
+        <v>0.625</v>
       </c>
     </row>
     <row customHeight="1" ht="17" r="17" s="50">
@@ -1874,16 +1874,16 @@
       </c>
       <c r="F21" s="87" t="inlineStr">
         <is>
-          <t>June 11, 2020</t>
+          <t>June 17, 2020</t>
         </is>
       </c>
       <c r="G21" s="88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H21" s="89" t="n"/>
       <c r="I21" s="90" t="inlineStr">
         <is>
-          <t>SL</t>
+          <t>VL</t>
         </is>
       </c>
     </row>
@@ -1900,10 +1900,20 @@
       <c r="D22" s="83" t="n">
         <v>0.416</v>
       </c>
-      <c r="F22" s="87" t="n"/>
-      <c r="G22" s="88" t="n"/>
+      <c r="F22" s="87" t="inlineStr">
+        <is>
+          <t>October 05, 2020</t>
+        </is>
+      </c>
+      <c r="G22" s="88" t="n">
+        <v>1</v>
+      </c>
       <c r="H22" s="89" t="n"/>
-      <c r="I22" s="90" t="n"/>
+      <c r="I22" s="90" t="inlineStr">
+        <is>
+          <t>VL</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15.8" r="23" s="50">
       <c r="A23" s="73" t="n">
@@ -1918,10 +1928,20 @@
       <c r="D23" s="83" t="n">
         <v>0.416</v>
       </c>
-      <c r="F23" s="87" t="n"/>
-      <c r="G23" s="88" t="n"/>
+      <c r="F23" s="87" t="inlineStr">
+        <is>
+          <t>June 23, 2020</t>
+        </is>
+      </c>
+      <c r="G23" s="88" t="n">
+        <v>1</v>
+      </c>
       <c r="H23" s="89" t="n"/>
-      <c r="I23" s="90" t="n"/>
+      <c r="I23" s="90" t="inlineStr">
+        <is>
+          <t>SL</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="15.8" r="24" s="50">
       <c r="A24" s="73" t="n">
@@ -1949,7 +1969,7 @@
         <v>43982</v>
       </c>
       <c r="C25" s="82" t="n">
-        <v>0</v>
+        <v>0.625</v>
       </c>
       <c r="D25" s="83" t="n">
         <v>0</v>
@@ -1970,7 +1990,7 @@
         <v>0</v>
       </c>
       <c r="D26" s="83" t="n">
-        <v>0</v>
+        <v>0.416</v>
       </c>
       <c r="F26" s="87" t="n"/>
       <c r="G26" s="88" t="n"/>
@@ -1985,7 +2005,7 @@
         <v>44012</v>
       </c>
       <c r="C27" s="82" t="n">
-        <v>0</v>
+        <v>0.625</v>
       </c>
       <c r="D27" s="83" t="n">
         <v>0</v>
@@ -2024,7 +2044,7 @@
         <v>0</v>
       </c>
       <c r="D29" s="83" t="n">
-        <v>0</v>
+        <v>0.416</v>
       </c>
       <c r="F29" s="87" t="n"/>
       <c r="G29" s="88" t="n"/>
@@ -2039,7 +2059,7 @@
         <v>44058</v>
       </c>
       <c r="C30" s="82" t="n">
-        <v>0</v>
+        <v>0.625</v>
       </c>
       <c r="D30" s="83" t="n">
         <v>0</v>
@@ -2078,7 +2098,7 @@
         <v>0</v>
       </c>
       <c r="D32" s="83" t="n">
-        <v>0</v>
+        <v>0.416</v>
       </c>
       <c r="F32" s="87" t="n"/>
       <c r="G32" s="88" t="n"/>
@@ -2093,7 +2113,7 @@
         <v>44104</v>
       </c>
       <c r="C33" s="82" t="n">
-        <v>0</v>
+        <v>0.625</v>
       </c>
       <c r="D33" s="83" t="n">
         <v>0</v>
@@ -2219,10 +2239,10 @@
         </is>
       </c>
       <c r="C40" s="93" t="n">
-        <v>5.625</v>
+        <v>29.125</v>
       </c>
       <c r="D40" s="94" t="n">
-        <v>3.744</v>
+        <v>26.201</v>
       </c>
       <c r="F40" s="95" t="n"/>
       <c r="G40" s="96" t="n"/>
@@ -2230,101 +2250,56 @@
       <c r="I40" s="98" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="C41" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="C42" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr"/>
-      <c r="B43" t="inlineStr"/>
-      <c r="C43" t="inlineStr"/>
-      <c r="D43" t="inlineStr"/>
-      <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>Contract Evaluation Date:</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>August 24, 2019 to August 24, 2020</t>
-        </is>
+      <c r="C43" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr"/>
-      <c r="B44" t="inlineStr"/>
-      <c r="C44" t="inlineStr"/>
-      <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr"/>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>Offense Name</t>
-        </is>
+      <c r="C44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr"/>
-      <c r="B45" t="inlineStr"/>
-      <c r="C45" t="inlineStr"/>
-      <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr"/>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>April 14, 2020</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>Late</t>
-        </is>
+      <c r="C45" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr"/>
-      <c r="B46" t="inlineStr"/>
-      <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr"/>
-      <c r="E46" t="inlineStr"/>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>June 10, 2020</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>No Time-in</t>
+      <c r="A46" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr"/>
-      <c r="B47" t="inlineStr"/>
-      <c r="C47" t="inlineStr"/>
-      <c r="D47" t="inlineStr"/>
-      <c r="E47" t="inlineStr"/>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>June 16, 2020</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>No Time-in</t>
+      <c r="A47" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
@@ -2336,66 +2311,46 @@
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr">
         <is>
-          <t>June 09, 2020</t>
+          <t>Contract Evaluation Date:</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
+          <t>August 30, 2019 to August 30, 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr"/>
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" t="inlineStr"/>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Offense Name</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr"/>
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr"/>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>June 10, 2020</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
           <t>No Time-in</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
@@ -2407,81 +2362,46 @@
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Prepared By: </t>
+          <t>June 16, 2020</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>Verified By:</t>
-        </is>
-      </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>Received By:</t>
+          <t>No Time-in</t>
         </is>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
+      <c r="A52" t="inlineStr"/>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr"/>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>June 09, 2020</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>No Time-in</t>
         </is>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
+      <c r="A53" t="inlineStr"/>
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="inlineStr"/>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>June 16, 2020</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Late</t>
         </is>
       </c>
     </row>
@@ -2493,27 +2413,12 @@
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Letecia Bodiongan</t>
+          <t>April 05, 2020</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>Susan Benjamin</t>
-        </is>
-      </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="J54" t="inlineStr">
-        <is>
-          <t>George Smith</t>
+          <t>No Time-out</t>
         </is>
       </c>
     </row>
@@ -2525,25 +2430,231 @@
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr">
         <is>
+          <t>June 30, 2020</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Late</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr"/>
+      <c r="B56" t="inlineStr"/>
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="inlineStr"/>
+      <c r="E56" t="inlineStr"/>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>June 23, 2020</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>No Time-in</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr"/>
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr"/>
+      <c r="E59" t="inlineStr"/>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prepared By: </t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>Verified By:</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>Received By:</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr"/>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Letecia Bodiongan</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>Susan Benjamin</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>George Smith</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr"/>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="inlineStr">
+        <is>
           <t>Accounting Supervisor - B</t>
         </is>
       </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="H55" t="inlineStr">
+      <c r="G63" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
         <is>
           <t>Finance and Admin Director</t>
         </is>
       </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="J55" t="inlineStr">
+      <c r="I63" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
         <is>
           <t>Employee</t>
         </is>

</xml_diff>